<commit_message>
Checked in on 1/22/22
</commit_message>
<xml_diff>
--- a/RADTestData/EmailNoMatch.xlsx
+++ b/RADTestData/EmailNoMatch.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="73">
   <si>
     <t>Execute</t>
   </si>
@@ -163,6 +163,96 @@
   </si>
   <si>
     <t>Wed Oct 27 17:08:39 EDT 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 01 10:48:17 EDT 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 01 10:48:27 EDT 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 01 10:48:37 EDT 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 01 10:48:48 EDT 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 01 10:48:57 EDT 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 01 10:49:09 EDT 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 05 18:16:30 EDT 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 05 18:16:40 EDT 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 05 18:16:50 EDT 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 05 18:17:00 EDT 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 05 18:17:10 EDT 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 05 18:17:20 EDT 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 12:15:51 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 12:16:01 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 12:16:11 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 12:16:20 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 12:16:30 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 12:16:40 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 22:15:59 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 22:16:11 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 22:16:20 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 22:16:30 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 22:16:40 EST 2021</t>
+  </si>
+  <si>
+    <t>Mon Nov 08 22:16:50 EST 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 19 10:48:40 EST 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 19 10:48:50 EST 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 19 10:49:00 EST 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 19 10:49:10 EST 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 19 10:49:20 EST 2021</t>
+  </si>
+  <si>
+    <t>Fri Nov 19 10:49:30 EST 2021</t>
   </si>
 </sst>
 </file>
@@ -548,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -562,7 +652,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -576,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -590,7 +680,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -604,7 +694,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -618,7 +708,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>

</xml_diff>